<commit_message>
heat transfer updates and bug fixes
heat transfer updates and bug fixes
</commit_message>
<xml_diff>
--- a/partgenout.xlsx
+++ b/partgenout.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
-    <workbookView activeTab="0" autoFilterDateGrouping="1" firstSheet="0" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="600" visibility="visible" windowHeight="8994" windowWidth="17280" xWindow="1464" yWindow="1464"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="1464" yWindow="1464" windowWidth="17280" windowHeight="8994" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
@@ -43,15 +43,15 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle builtinId="0" name="Normal" xfId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium2"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
 </styleSheet>
 </file>
 
@@ -364,7 +364,7 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="14.4"/>
   <cols>
-    <col customWidth="1" max="1" min="1" width="14.3671875"/>
+    <col width="14.3671875" customWidth="1" min="1" max="1"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -392,7 +392,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>0.005537469539251676</t>
+          <t>0.007148449489526548</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
@@ -409,7 +409,7 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>19.25</t>
+          <t>19.0</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
@@ -426,7 +426,7 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>0.00037563259962332434</t>
+          <t>0.0006320705701557373</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
@@ -443,7 +443,7 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>0.17720546041406252</t>
+          <t>5.179405571978401</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
@@ -460,7 +460,7 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>9.628360634016016e-05</t>
+          <t>0.00016045503652754083</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
@@ -477,7 +477,7 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>30.0</t>
+          <t>59.0</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
@@ -494,7 +494,7 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>9.25</t>
+          <t>9.5</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
@@ -504,6 +504,6 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>